<commit_message>
Custom power plant calcs
</commit_message>
<xml_diff>
--- a/data/power-plants/mdg-power-plants.xlsx
+++ b/data/power-plants/mdg-power-plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/repositories/tza-V20/data/power-plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE07FF6-5634-1B43-ADF7-1D6558A137F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0686B1-D93C-B14B-BC0C-C4A44360547A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{9189665D-D17D-EF4D-85B0-DA83D4B48E95}"/>
   </bookViews>
@@ -661,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D774F4-2765-A540-807C-E0B9ADB9B465}">
-  <dimension ref="A1:BF60"/>
+  <dimension ref="A1:BH60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="BA33" sqref="BA33:BF40"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="BH2" sqref="BH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,7 +691,7 @@
     <col min="58" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
@@ -1056,8 +1056,12 @@
         <f t="shared" si="2"/>
         <v>2023: 0</v>
       </c>
-    </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+      <c r="BH2" s="2">
+        <f>822/(AT2*8760/1000)</f>
+        <v>0.13190275012420041</v>
+      </c>
+    </row>
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
@@ -1259,7 +1263,7 @@
         <v>2024: 0</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -1461,7 +1465,7 @@
         <v>2025: 0</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1663,7 +1667,7 @@
         <v>2026: 0</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
@@ -1865,7 +1869,7 @@
         <v>2027: 0</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>2028: 0</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>11</v>
       </c>
@@ -2183,7 +2187,7 @@
         <v>2029: 0</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
@@ -2299,7 +2303,7 @@
         <v>2030: 0</v>
       </c>
     </row>
-    <row r="10" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:60" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>11</v>
       </c>
@@ -2473,7 +2477,7 @@
         <v>2031: 0</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>11</v>
       </c>
@@ -2675,7 +2679,7 @@
         <v>2032: 0</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
@@ -2877,7 +2881,7 @@
         <v>2033: 0</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
@@ -3079,7 +3083,7 @@
         <v>2034: 0</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>11</v>
       </c>
@@ -3281,7 +3285,7 @@
         <v>2035: 0</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>11</v>
       </c>
@@ -3483,7 +3487,7 @@
         <v>2036: 0</v>
       </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
All data except costs
</commit_message>
<xml_diff>
--- a/data/power-plants/mdg-power-plants.xlsx
+++ b/data/power-plants/mdg-power-plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/repositories/tza-V20/data/power-plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC17A90-4F9A-D749-B711-42FC8E0FD14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188E0176-95BE-6547-92A2-0C4081D2F472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{9189665D-D17D-EF4D-85B0-DA83D4B48E95}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{9189665D-D17D-EF4D-85B0-DA83D4B48E95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="66">
   <si>
     <t>Country</t>
   </si>
@@ -244,7 +244,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="174" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,6 +267,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,10 +326,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,9 +351,11 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5527,13 +5540,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE914C88-47AD-0D4D-AE5A-79EF48B67CC9}">
   <dimension ref="A2:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="12" width="10.83203125" style="2"/>
+    <col min="13" max="13" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
@@ -5953,6 +5968,21 @@
       <c r="D8" s="9" t="s">
         <v>64</v>
       </c>
+      <c r="F8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2023</v>
+      </c>
+      <c r="L8" s="2">
+        <v>25.98</v>
+      </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
@@ -5970,13 +6000,35 @@
         <f t="shared" si="10"/>
         <v>1.53</v>
       </c>
+      <c r="F9" s="2" t="str">
+        <f>$A9&amp;": "&amp;ROUND(B9,2)</f>
+        <v>2024: 1.53</v>
+      </c>
+      <c r="G9" s="2" t="str">
+        <f t="shared" ref="G9:H9" si="11">$A9&amp;": "&amp;ROUND(C9,2)</f>
+        <v>2024: 1.53</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>2024: 1.53</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2024</v>
+      </c>
+      <c r="L9" s="2">
+        <v>27.72</v>
+      </c>
+      <c r="M9" s="12">
+        <f>L9/L8-1</f>
+        <v>6.6974595842955953E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>2025</v>
       </c>
       <c r="B10" s="11">
-        <f t="shared" ref="B10:D35" si="11">INDEX($B$3:$AB$5,MATCH(B$8,$A$3:$A$5,0),MATCH($A10,$B$2:$AB$2,0))</f>
+        <f t="shared" ref="B10:D35" si="12">INDEX($B$3:$AB$5,MATCH(B$8,$A$3:$A$5,0),MATCH($A10,$B$2:$AB$2,0))</f>
         <v>1.62</v>
       </c>
       <c r="C10" s="11">
@@ -5987,13 +6039,35 @@
         <f t="shared" si="10"/>
         <v>1.59</v>
       </c>
+      <c r="F10" s="2" t="str">
+        <f t="shared" ref="F10:F35" si="13">$A10&amp;": "&amp;ROUND(B10,2)</f>
+        <v>2025: 1.62</v>
+      </c>
+      <c r="G10" s="2" t="str">
+        <f t="shared" ref="G10:G35" si="14">$A10&amp;": "&amp;ROUND(C10,2)</f>
+        <v>2025: 1.6</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f t="shared" ref="H10:H35" si="15">$A10&amp;": "&amp;ROUND(D10,2)</f>
+        <v>2025: 1.59</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2025</v>
+      </c>
+      <c r="L10" s="2">
+        <v>29.46</v>
+      </c>
+      <c r="M10" s="12">
+        <f t="shared" ref="M10:M35" si="16">L10/L9-1</f>
+        <v>6.277056277056281E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>2026</v>
       </c>
       <c r="B11" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6840000000000002</v>
       </c>
       <c r="C11" s="11">
@@ -6004,13 +6078,35 @@
         <f t="shared" si="10"/>
         <v>1.6</v>
       </c>
+      <c r="F11" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2026: 1.68</v>
+      </c>
+      <c r="G11" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2026: 1.64</v>
+      </c>
+      <c r="H11" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2026: 1.6</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2026</v>
+      </c>
+      <c r="L11" s="2">
+        <v>31.56</v>
+      </c>
+      <c r="M11" s="12">
+        <f t="shared" si="16"/>
+        <v>7.1283095723014167E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>2027</v>
       </c>
       <c r="B12" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.748</v>
       </c>
       <c r="C12" s="11">
@@ -6021,13 +6117,35 @@
         <f t="shared" si="10"/>
         <v>1.61</v>
       </c>
+      <c r="F12" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2027: 1.75</v>
+      </c>
+      <c r="G12" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2027: 1.68</v>
+      </c>
+      <c r="H12" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2027: 1.61</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2027</v>
+      </c>
+      <c r="L12" s="2">
+        <v>33.659999999999997</v>
+      </c>
+      <c r="M12" s="12">
+        <f t="shared" si="16"/>
+        <v>6.6539923954372471E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>2028</v>
       </c>
       <c r="B13" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.8120000000000001</v>
       </c>
       <c r="C13" s="11">
@@ -6038,13 +6156,35 @@
         <f t="shared" si="10"/>
         <v>1.6199999999999999</v>
       </c>
+      <c r="F13" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2028: 1.81</v>
+      </c>
+      <c r="G13" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2028: 1.73</v>
+      </c>
+      <c r="H13" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2028: 1.62</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2028</v>
+      </c>
+      <c r="L13" s="2">
+        <v>35.76</v>
+      </c>
+      <c r="M13" s="12">
+        <f t="shared" si="16"/>
+        <v>6.2388591800356608E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>2029</v>
       </c>
       <c r="B14" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.8759999999999999</v>
       </c>
       <c r="C14" s="11">
@@ -6055,13 +6195,35 @@
         <f t="shared" si="10"/>
         <v>1.63</v>
       </c>
+      <c r="F14" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2029: 1.88</v>
+      </c>
+      <c r="G14" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2029: 1.77</v>
+      </c>
+      <c r="H14" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2029: 1.63</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2029</v>
+      </c>
+      <c r="L14" s="2">
+        <v>37.86</v>
+      </c>
+      <c r="M14" s="12">
+        <f t="shared" si="16"/>
+        <v>5.8724832214765099E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>2030</v>
       </c>
       <c r="B15" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.94</v>
       </c>
       <c r="C15" s="11">
@@ -6072,13 +6234,35 @@
         <f t="shared" si="10"/>
         <v>1.64</v>
       </c>
+      <c r="F15" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2030: 1.94</v>
+      </c>
+      <c r="G15" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2030: 1.81</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2030: 1.64</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2030</v>
+      </c>
+      <c r="L15" s="2">
+        <v>39.96</v>
+      </c>
+      <c r="M15" s="12">
+        <f t="shared" si="16"/>
+        <v>5.5467511885895382E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>2031</v>
       </c>
       <c r="B16" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.98</v>
       </c>
       <c r="C16" s="11">
@@ -6089,13 +6273,35 @@
         <f t="shared" si="10"/>
         <v>1.5939999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2031: 1.98</v>
+      </c>
+      <c r="G16" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2031: 1.81</v>
+      </c>
+      <c r="H16" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2031: 1.59</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2031</v>
+      </c>
+      <c r="L16" s="2">
+        <v>42.41</v>
+      </c>
+      <c r="M16" s="12">
+        <f t="shared" si="16"/>
+        <v>6.131131131131129E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>2032</v>
       </c>
       <c r="B17" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.02</v>
       </c>
       <c r="C17" s="11">
@@ -6106,13 +6312,35 @@
         <f t="shared" si="10"/>
         <v>1.5479999999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2032: 2.02</v>
+      </c>
+      <c r="G17" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2032: 1.81</v>
+      </c>
+      <c r="H17" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2032: 1.55</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2032</v>
+      </c>
+      <c r="L17" s="2">
+        <v>44.87</v>
+      </c>
+      <c r="M17" s="12">
+        <f t="shared" si="16"/>
+        <v>5.8005187455788754E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>2033</v>
       </c>
       <c r="B18" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.06</v>
       </c>
       <c r="C18" s="11">
@@ -6123,13 +6351,35 @@
         <f t="shared" si="10"/>
         <v>1.502</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2033: 2.06</v>
+      </c>
+      <c r="G18" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2033: 1.82</v>
+      </c>
+      <c r="H18" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2033: 1.5</v>
+      </c>
+      <c r="K18" s="2">
+        <v>2033</v>
+      </c>
+      <c r="L18" s="2">
+        <v>47.32</v>
+      </c>
+      <c r="M18" s="12">
+        <f t="shared" si="16"/>
+        <v>5.4602184087363614E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>2034</v>
       </c>
       <c r="B19" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.1</v>
       </c>
       <c r="C19" s="11">
@@ -6140,13 +6390,35 @@
         <f t="shared" si="10"/>
         <v>1.456</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2034: 2.1</v>
+      </c>
+      <c r="G19" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2034: 1.82</v>
+      </c>
+      <c r="H19" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2034: 1.46</v>
+      </c>
+      <c r="K19" s="2">
+        <v>2034</v>
+      </c>
+      <c r="L19" s="2">
+        <v>49.77</v>
+      </c>
+      <c r="M19" s="12">
+        <f t="shared" si="16"/>
+        <v>5.177514792899407E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>2035</v>
       </c>
       <c r="B20" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.14</v>
       </c>
       <c r="C20" s="11">
@@ -6157,13 +6429,35 @@
         <f t="shared" si="10"/>
         <v>1.41</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2035: 2.14</v>
+      </c>
+      <c r="G20" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2035: 1.82</v>
+      </c>
+      <c r="H20" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2035: 1.41</v>
+      </c>
+      <c r="K20" s="2">
+        <v>2035</v>
+      </c>
+      <c r="L20" s="2">
+        <v>52.22</v>
+      </c>
+      <c r="M20" s="12">
+        <f t="shared" si="16"/>
+        <v>4.9226441631504914E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>2036</v>
       </c>
       <c r="B21" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.1800000000000002</v>
       </c>
       <c r="C21" s="11">
@@ -6174,13 +6468,35 @@
         <f t="shared" si="10"/>
         <v>1.3419999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2036: 2.18</v>
+      </c>
+      <c r="G21" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2036: 1.81</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2036: 1.34</v>
+      </c>
+      <c r="K21" s="2">
+        <v>2036</v>
+      </c>
+      <c r="L21" s="2">
+        <v>55.14</v>
+      </c>
+      <c r="M21" s="12">
+        <f t="shared" si="16"/>
+        <v>5.5917273075450025E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>2037</v>
       </c>
       <c r="B22" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.2200000000000002</v>
       </c>
       <c r="C22" s="11">
@@ -6191,13 +6507,35 @@
         <f t="shared" si="10"/>
         <v>1.274</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2037: 2.22</v>
+      </c>
+      <c r="G22" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2037: 1.8</v>
+      </c>
+      <c r="H22" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2037: 1.27</v>
+      </c>
+      <c r="K22" s="2">
+        <v>2037</v>
+      </c>
+      <c r="L22" s="2">
+        <v>58.05</v>
+      </c>
+      <c r="M22" s="12">
+        <f t="shared" si="16"/>
+        <v>5.277475516866148E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>2038</v>
       </c>
       <c r="B23" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.2599999999999998</v>
       </c>
       <c r="C23" s="11">
@@ -6208,13 +6546,35 @@
         <f t="shared" si="10"/>
         <v>1.206</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2038: 2.26</v>
+      </c>
+      <c r="G23" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2038: 1.8</v>
+      </c>
+      <c r="H23" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2038: 1.21</v>
+      </c>
+      <c r="K23" s="2">
+        <v>2038</v>
+      </c>
+      <c r="L23" s="2">
+        <v>60.97</v>
+      </c>
+      <c r="M23" s="12">
+        <f t="shared" si="16"/>
+        <v>5.0301464254952633E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>2039</v>
       </c>
       <c r="B24" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="C24" s="11">
@@ -6225,195 +6585,460 @@
         <f t="shared" si="10"/>
         <v>1.1379999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F24" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2039: 2.3</v>
+      </c>
+      <c r="G24" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2039: 1.79</v>
+      </c>
+      <c r="H24" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2039: 1.14</v>
+      </c>
+      <c r="K24" s="2">
+        <v>2039</v>
+      </c>
+      <c r="L24" s="2">
+        <v>63.89</v>
+      </c>
+      <c r="M24" s="12">
+        <f t="shared" si="16"/>
+        <v>4.7892406101361251E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>2040</v>
       </c>
       <c r="B25" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.34</v>
       </c>
       <c r="C25" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.78</v>
       </c>
       <c r="D25" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.07</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2040: 2.34</v>
+      </c>
+      <c r="G25" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2040: 1.78</v>
+      </c>
+      <c r="H25" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2040: 1.07</v>
+      </c>
+      <c r="K25" s="2">
+        <v>2040</v>
+      </c>
+      <c r="L25" s="2">
+        <v>66.8</v>
+      </c>
+      <c r="M25" s="12">
+        <f t="shared" si="16"/>
+        <v>4.5547033964626671E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>2041</v>
       </c>
       <c r="B26" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.3759999999999999</v>
       </c>
       <c r="C26" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.772</v>
       </c>
       <c r="D26" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.006</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F26" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2041: 2.38</v>
+      </c>
+      <c r="G26" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2041: 1.77</v>
+      </c>
+      <c r="H26" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2041: 1.01</v>
+      </c>
+      <c r="K26" s="2">
+        <v>2041</v>
+      </c>
+      <c r="L26" s="2">
+        <v>70.25</v>
+      </c>
+      <c r="M26" s="12">
+        <f t="shared" si="16"/>
+        <v>5.1646706586826463E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>2042</v>
       </c>
       <c r="B27" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.4119999999999999</v>
       </c>
       <c r="C27" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.764</v>
       </c>
       <c r="D27" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.94200000000000006</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F27" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2042: 2.41</v>
+      </c>
+      <c r="G27" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2042: 1.76</v>
+      </c>
+      <c r="H27" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2042: 0.94</v>
+      </c>
+      <c r="K27" s="2">
+        <v>2042</v>
+      </c>
+      <c r="L27" s="2">
+        <v>73.69</v>
+      </c>
+      <c r="M27" s="12">
+        <f t="shared" si="16"/>
+        <v>4.8967971530249121E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>2043</v>
       </c>
       <c r="B28" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.448</v>
       </c>
       <c r="C28" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.756</v>
       </c>
       <c r="D28" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.878</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F28" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2043: 2.45</v>
+      </c>
+      <c r="G28" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2043: 1.76</v>
+      </c>
+      <c r="H28" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2043: 0.88</v>
+      </c>
+      <c r="K28" s="2">
+        <v>2043</v>
+      </c>
+      <c r="L28" s="2">
+        <v>77.13</v>
+      </c>
+      <c r="M28" s="12">
+        <f t="shared" si="16"/>
+        <v>4.6682046410639222E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>2044</v>
       </c>
       <c r="B29" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.484</v>
       </c>
       <c r="C29" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.748</v>
       </c>
       <c r="D29" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.81400000000000006</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F29" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2044: 2.48</v>
+      </c>
+      <c r="G29" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2044: 1.75</v>
+      </c>
+      <c r="H29" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2044: 0.81</v>
+      </c>
+      <c r="K29" s="2">
+        <v>2044</v>
+      </c>
+      <c r="L29" s="2">
+        <v>80.569999999999993</v>
+      </c>
+      <c r="M29" s="12">
+        <f t="shared" si="16"/>
+        <v>4.46000259302477E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
         <v>2045</v>
       </c>
       <c r="B30" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.52</v>
       </c>
       <c r="C30" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.74</v>
       </c>
       <c r="D30" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F30" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2045: 2.52</v>
+      </c>
+      <c r="G30" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2045: 1.74</v>
+      </c>
+      <c r="H30" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2045: 0.75</v>
+      </c>
+      <c r="K30" s="2">
+        <v>2045</v>
+      </c>
+      <c r="L30" s="2">
+        <v>84.02</v>
+      </c>
+      <c r="M30" s="12">
+        <f t="shared" si="16"/>
+        <v>4.2819908154399844E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>2046</v>
       </c>
       <c r="B31" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.5680000000000001</v>
       </c>
       <c r="C31" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.734</v>
       </c>
       <c r="D31" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.70599999999999996</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F31" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2046: 2.57</v>
+      </c>
+      <c r="G31" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2046: 1.73</v>
+      </c>
+      <c r="H31" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2046: 0.71</v>
+      </c>
+      <c r="K31" s="2">
+        <v>2046</v>
+      </c>
+      <c r="L31" s="2">
+        <v>87.98</v>
+      </c>
+      <c r="M31" s="12">
+        <f t="shared" si="16"/>
+        <v>4.7131635324922705E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>2047</v>
       </c>
       <c r="B32" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.6160000000000001</v>
       </c>
       <c r="C32" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.728</v>
       </c>
       <c r="D32" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.66200000000000003</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2047: 2.62</v>
+      </c>
+      <c r="G32" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2047: 1.73</v>
+      </c>
+      <c r="H32" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2047: 0.66</v>
+      </c>
+      <c r="K32" s="2">
+        <v>2047</v>
+      </c>
+      <c r="L32" s="2">
+        <v>91.94</v>
+      </c>
+      <c r="M32" s="12">
+        <f t="shared" si="16"/>
+        <v>4.5010229597635787E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>2048</v>
       </c>
       <c r="B33" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.6639999999999997</v>
       </c>
       <c r="C33" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.722</v>
       </c>
       <c r="D33" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.61799999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F33" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2048: 2.66</v>
+      </c>
+      <c r="G33" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2048: 1.72</v>
+      </c>
+      <c r="H33" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2048: 0.62</v>
+      </c>
+      <c r="K33" s="2">
+        <v>2048</v>
+      </c>
+      <c r="L33" s="2">
+        <v>95.9</v>
+      </c>
+      <c r="M33" s="12">
+        <f t="shared" si="16"/>
+        <v>4.3071568414183359E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>2049</v>
       </c>
       <c r="B34" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7119999999999997</v>
       </c>
       <c r="C34" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.716</v>
       </c>
       <c r="D34" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.57400000000000007</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F34" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2049: 2.71</v>
+      </c>
+      <c r="G34" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2049: 1.72</v>
+      </c>
+      <c r="H34" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2049: 0.57</v>
+      </c>
+      <c r="K34" s="2">
+        <v>2049</v>
+      </c>
+      <c r="L34" s="2">
+        <v>99.87</v>
+      </c>
+      <c r="M34" s="12">
+        <f t="shared" si="16"/>
+        <v>4.1397288842544233E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>2050</v>
       </c>
       <c r="B35" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.76</v>
       </c>
       <c r="C35" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.71</v>
       </c>
       <c r="D35" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.53</v>
+      </c>
+      <c r="F35" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>2050: 2.76</v>
+      </c>
+      <c r="G35" s="2" t="str">
+        <f t="shared" si="14"/>
+        <v>2050: 1.71</v>
+      </c>
+      <c r="H35" s="2" t="str">
+        <f t="shared" si="15"/>
+        <v>2050: 0.53</v>
+      </c>
+      <c r="K35" s="2">
+        <v>2050</v>
+      </c>
+      <c r="L35" s="2">
+        <v>103.83</v>
+      </c>
+      <c r="M35" s="12">
+        <f t="shared" si="16"/>
+        <v>3.9651547011114285E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed capacity factor min issue and updated hydro capacity
</commit_message>
<xml_diff>
--- a/data/power-plants/mdg-power-plants.xlsx
+++ b/data/power-plants/mdg-power-plants.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/repositories/tza-V20/data/power-plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188E0176-95BE-6547-92A2-0C4081D2F472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FAAAB5-7637-904E-B2F8-A380F6DD05B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{9189665D-D17D-EF4D-85B0-DA83D4B48E95}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{9189665D-D17D-EF4D-85B0-DA83D4B48E95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$K$1</definedName>
@@ -245,7 +246,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -330,7 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -351,7 +352,10 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D774F4-2765-A540-807C-E0B9ADB9B465}">
   <dimension ref="A1:BF60"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="BI4" sqref="BI4:BI10"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,122 +925,122 @@
       </c>
       <c r="O2" s="5">
         <f>SUMIFS($E$2:$E$26,$F$2:$F$26,$N2,$I$2:$I$26,"&lt;="&amp;DATE(O$1,1,1),$J$2:$J$26,"&gt;="&amp;DATE(O$1,1,1),$H$2:$H$26,"operating")</f>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="P2" s="5">
         <f t="shared" ref="P2:AP7" si="0">SUMIFS($E$2:$E$26,$F$2:$F$26,$N2,$I$2:$I$26,"&lt;="&amp;DATE(P$1,1,1),$J$2:$J$26,"&gt;="&amp;DATE(P$1,1,1),$H$2:$H$26,"operating")</f>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="Q2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="R2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="S2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="T2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="U2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="V2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="W2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="X2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="Y2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="Z2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AA2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AB2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AC2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AD2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AE2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AF2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AG2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AH2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AI2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AJ2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AK2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AL2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AM2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AN2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AO2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AP2" s="5">
         <f t="shared" si="0"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AS2" s="10">
         <v>2023</v>
       </c>
       <c r="AT2" s="8">
         <f>INDEX($O$2:$AP$7,MATCH(AT$1,$N$2:$N$7,0),MATCH($AS2,$O$1:$AP$1,0))</f>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU2" s="8">
         <f t="shared" ref="AU2:AY17" si="1">INDEX($O$2:$AP$7,MATCH(AU$1,$N$2:$N$7,0),MATCH($AS2,$O$1:$AP$1,0))</f>
@@ -1060,7 +1064,7 @@
       </c>
       <c r="BA2" s="2" t="str">
         <f>$AS2&amp;": "&amp;ROUND(AT2/1000,3)</f>
-        <v>2023: 0.711</v>
+        <v>2023: 0.152</v>
       </c>
       <c r="BB2" s="2" t="str">
         <f t="shared" ref="BB2:BF2" si="2">$AS2&amp;": "&amp;ROUND(AU2/1000,3)</f>
@@ -1238,7 +1242,7 @@
       </c>
       <c r="AT3" s="8">
         <f t="shared" ref="AT3:AY29" si="5">INDEX($O$2:$AP$7,MATCH(AT$1,$N$2:$N$7,0),MATCH($AS3,$O$1:$AP$1,0))</f>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU3" s="8">
         <f t="shared" si="1"/>
@@ -1262,7 +1266,7 @@
       </c>
       <c r="BA3" s="2" t="str">
         <f t="shared" ref="BA3:BA29" si="6">$AS3&amp;": "&amp;ROUND(AT3/1000,3)</f>
-        <v>2024: 0.711</v>
+        <v>2024: 0.152</v>
       </c>
       <c r="BB3" s="2" t="str">
         <f t="shared" ref="BB3:BB29" si="7">$AS3&amp;": "&amp;ROUND(AU3/1000,3)</f>
@@ -1440,7 +1444,7 @@
       </c>
       <c r="AT4" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU4" s="8">
         <f t="shared" si="1"/>
@@ -1464,7 +1468,7 @@
       </c>
       <c r="BA4" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2025: 0.711</v>
+        <v>2025: 0.152</v>
       </c>
       <c r="BB4" s="2" t="str">
         <f t="shared" si="7"/>
@@ -1642,7 +1646,7 @@
       </c>
       <c r="AT5" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU5" s="8">
         <f t="shared" si="1"/>
@@ -1666,7 +1670,7 @@
       </c>
       <c r="BA5" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2026: 0.711</v>
+        <v>2026: 0.152</v>
       </c>
       <c r="BB5" s="2" t="str">
         <f t="shared" si="7"/>
@@ -1703,7 +1707,7 @@
         <v>32</v>
       </c>
       <c r="E6" s="3">
-        <v>560</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>23</v>
@@ -1844,7 +1848,7 @@
       </c>
       <c r="AT6" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU6" s="8">
         <f t="shared" si="1"/>
@@ -1868,7 +1872,7 @@
       </c>
       <c r="BA6" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2027: 0.711</v>
+        <v>2027: 0.152</v>
       </c>
       <c r="BB6" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2046,7 +2050,7 @@
       </c>
       <c r="AT7" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU7" s="8">
         <f t="shared" si="1"/>
@@ -2070,7 +2074,7 @@
       </c>
       <c r="BA7" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2028: 0.711</v>
+        <v>2028: 0.152</v>
       </c>
       <c r="BB7" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2162,7 +2166,7 @@
       </c>
       <c r="AT8" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU8" s="8">
         <f t="shared" si="1"/>
@@ -2186,7 +2190,7 @@
       </c>
       <c r="BA8" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2029: 0.711</v>
+        <v>2029: 0.152</v>
       </c>
       <c r="BB8" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2278,7 +2282,7 @@
       </c>
       <c r="AT9" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU9" s="8">
         <f t="shared" si="1"/>
@@ -2302,7 +2306,7 @@
       </c>
       <c r="BA9" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2030: 0.711</v>
+        <v>2030: 0.152</v>
       </c>
       <c r="BB9" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2452,7 +2456,7 @@
       </c>
       <c r="AT10" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU10" s="8">
         <f t="shared" si="1"/>
@@ -2476,7 +2480,7 @@
       </c>
       <c r="BA10" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2031: 0.711</v>
+        <v>2031: 0.152</v>
       </c>
       <c r="BB10" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2654,7 +2658,7 @@
       </c>
       <c r="AT11" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU11" s="8">
         <f t="shared" si="1"/>
@@ -2678,7 +2682,7 @@
       </c>
       <c r="BA11" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2032: 0.711</v>
+        <v>2032: 0.152</v>
       </c>
       <c r="BB11" s="2" t="str">
         <f t="shared" si="7"/>
@@ -2856,7 +2860,7 @@
       </c>
       <c r="AT12" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU12" s="8">
         <f t="shared" si="1"/>
@@ -2880,7 +2884,7 @@
       </c>
       <c r="BA12" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2033: 0.711</v>
+        <v>2033: 0.152</v>
       </c>
       <c r="BB12" s="2" t="str">
         <f t="shared" si="7"/>
@@ -3058,7 +3062,7 @@
       </c>
       <c r="AT13" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU13" s="8">
         <f t="shared" si="1"/>
@@ -3082,7 +3086,7 @@
       </c>
       <c r="BA13" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2034: 0.711</v>
+        <v>2034: 0.152</v>
       </c>
       <c r="BB13" s="2" t="str">
         <f t="shared" si="7"/>
@@ -3260,7 +3264,7 @@
       </c>
       <c r="AT14" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU14" s="8">
         <f t="shared" si="1"/>
@@ -3284,7 +3288,7 @@
       </c>
       <c r="BA14" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2035: 0.711</v>
+        <v>2035: 0.152</v>
       </c>
       <c r="BB14" s="2" t="str">
         <f t="shared" si="7"/>
@@ -3462,7 +3466,7 @@
       </c>
       <c r="AT15" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU15" s="8">
         <f t="shared" si="1"/>
@@ -3486,7 +3490,7 @@
       </c>
       <c r="BA15" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2036: 0.711</v>
+        <v>2036: 0.152</v>
       </c>
       <c r="BB15" s="2" t="str">
         <f t="shared" si="7"/>
@@ -3664,7 +3668,7 @@
       </c>
       <c r="AT16" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU16" s="8">
         <f t="shared" si="1"/>
@@ -3688,7 +3692,7 @@
       </c>
       <c r="BA16" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2037: 0.711</v>
+        <v>2037: 0.152</v>
       </c>
       <c r="BB16" s="2" t="str">
         <f t="shared" si="7"/>
@@ -3778,7 +3782,7 @@
       </c>
       <c r="AT17" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU17" s="8">
         <f t="shared" si="1"/>
@@ -3802,7 +3806,7 @@
       </c>
       <c r="BA17" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2038: 0.711</v>
+        <v>2038: 0.152</v>
       </c>
       <c r="BB17" s="2" t="str">
         <f t="shared" si="7"/>
@@ -3892,7 +3896,7 @@
       </c>
       <c r="AT18" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU18" s="8">
         <f t="shared" si="5"/>
@@ -3916,7 +3920,7 @@
       </c>
       <c r="BA18" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2039: 0.711</v>
+        <v>2039: 0.152</v>
       </c>
       <c r="BB18" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4006,7 +4010,7 @@
       </c>
       <c r="AT19" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU19" s="8">
         <f t="shared" si="5"/>
@@ -4030,7 +4034,7 @@
       </c>
       <c r="BA19" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2040: 0.711</v>
+        <v>2040: 0.152</v>
       </c>
       <c r="BB19" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4120,7 +4124,7 @@
       </c>
       <c r="AT20" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU20" s="8">
         <f t="shared" si="5"/>
@@ -4144,7 +4148,7 @@
       </c>
       <c r="BA20" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2041: 0.711</v>
+        <v>2041: 0.152</v>
       </c>
       <c r="BB20" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4234,7 +4238,7 @@
       </c>
       <c r="AT21" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU21" s="8">
         <f t="shared" si="5"/>
@@ -4258,7 +4262,7 @@
       </c>
       <c r="BA21" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2042: 0.711</v>
+        <v>2042: 0.152</v>
       </c>
       <c r="BB21" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4348,7 +4352,7 @@
       </c>
       <c r="AT22" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU22" s="8">
         <f t="shared" si="5"/>
@@ -4372,7 +4376,7 @@
       </c>
       <c r="BA22" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2043: 0.711</v>
+        <v>2043: 0.152</v>
       </c>
       <c r="BB22" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4436,7 +4440,7 @@
       </c>
       <c r="AT23" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU23" s="8">
         <f t="shared" si="5"/>
@@ -4460,7 +4464,7 @@
       </c>
       <c r="BA23" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2044: 0.711</v>
+        <v>2044: 0.152</v>
       </c>
       <c r="BB23" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4524,7 +4528,7 @@
       </c>
       <c r="AT24" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU24" s="8">
         <f t="shared" si="5"/>
@@ -4548,7 +4552,7 @@
       </c>
       <c r="BA24" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2045: 0.711</v>
+        <v>2045: 0.152</v>
       </c>
       <c r="BB24" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4612,7 +4616,7 @@
       </c>
       <c r="AT25" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU25" s="8">
         <f t="shared" si="5"/>
@@ -4636,7 +4640,7 @@
       </c>
       <c r="BA25" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2046: 0.711</v>
+        <v>2046: 0.152</v>
       </c>
       <c r="BB25" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4700,7 +4704,7 @@
       </c>
       <c r="AT26" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU26" s="8">
         <f t="shared" si="5"/>
@@ -4724,7 +4728,7 @@
       </c>
       <c r="BA26" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2047: 0.711</v>
+        <v>2047: 0.152</v>
       </c>
       <c r="BB26" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4753,7 +4757,7 @@
       </c>
       <c r="AT27" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU27" s="8">
         <f t="shared" si="5"/>
@@ -4777,7 +4781,7 @@
       </c>
       <c r="BA27" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2048: 0.711</v>
+        <v>2048: 0.152</v>
       </c>
       <c r="BB27" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4806,7 +4810,7 @@
       </c>
       <c r="AT28" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU28" s="8">
         <f t="shared" si="5"/>
@@ -4830,7 +4834,7 @@
       </c>
       <c r="BA28" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2049: 0.711</v>
+        <v>2049: 0.152</v>
       </c>
       <c r="BB28" s="2" t="str">
         <f t="shared" si="7"/>
@@ -4859,7 +4863,7 @@
       </c>
       <c r="AT29" s="8">
         <f t="shared" si="5"/>
-        <v>711.4</v>
+        <v>151.96</v>
       </c>
       <c r="AU29" s="8">
         <f t="shared" si="5"/>
@@ -4883,7 +4887,7 @@
       </c>
       <c r="BA29" s="2" t="str">
         <f t="shared" si="6"/>
-        <v>2050: 0.711</v>
+        <v>2050: 0.152</v>
       </c>
       <c r="BB29" s="2" t="str">
         <f t="shared" si="7"/>
@@ -5540,8 +5544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE914C88-47AD-0D4D-AE5A-79EF48B67CC9}">
   <dimension ref="A2:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9:M35"/>
+    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7041,4 +7045,390 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9783DCC0-9729-EA44-8E9F-A8637A17B22B}">
+  <dimension ref="A2:D29"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+      <c r="B2">
+        <v>2023</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0.84</v>
+      </c>
+      <c r="D2" t="str">
+        <f>B2&amp;": "&amp;ROUND(C2,2)</f>
+        <v>2023: 0.84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3">
+        <v>2024</v>
+      </c>
+      <c r="C3" s="15">
+        <f>$C$2+(($C$29-$C$2)*($B3-$B$2)/($B$29-$B$2))</f>
+        <v>0.80888888888888888</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D29" si="0">B3&amp;": "&amp;ROUND(C3,2)</f>
+        <v>2024: 0.81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4">
+        <v>2025</v>
+      </c>
+      <c r="C4" s="15">
+        <f t="shared" ref="C4:C28" si="1">$C$2+(($C$29-$C$2)*($B4-$B$2)/($B$29-$B$2))</f>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>2025: 0.78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5">
+        <v>2026</v>
+      </c>
+      <c r="C5" s="15">
+        <f t="shared" si="1"/>
+        <v>0.74666666666666659</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>2026: 0.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
+      <c r="B6">
+        <v>2027</v>
+      </c>
+      <c r="C6" s="15">
+        <f t="shared" si="1"/>
+        <v>0.7155555555555555</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>2027: 0.72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+      <c r="B7">
+        <v>2028</v>
+      </c>
+      <c r="C7" s="15">
+        <f t="shared" si="1"/>
+        <v>0.68444444444444441</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>2028: 0.68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8">
+        <v>2029</v>
+      </c>
+      <c r="C8" s="15">
+        <f t="shared" si="1"/>
+        <v>0.65333333333333332</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>2029: 0.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="14"/>
+      <c r="B9">
+        <v>2030</v>
+      </c>
+      <c r="C9" s="15">
+        <f t="shared" si="1"/>
+        <v>0.62222222222222223</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>2030: 0.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>2031</v>
+      </c>
+      <c r="C10" s="15">
+        <f t="shared" si="1"/>
+        <v>0.59111111111111114</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>2031: 0.59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>2032</v>
+      </c>
+      <c r="C11" s="15">
+        <f t="shared" si="1"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>2032: 0.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>2033</v>
+      </c>
+      <c r="C12" s="15">
+        <f t="shared" si="1"/>
+        <v>0.52888888888888885</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>2033: 0.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>2034</v>
+      </c>
+      <c r="C13" s="15">
+        <f t="shared" si="1"/>
+        <v>0.49777777777777776</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>2034: 0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>2035</v>
+      </c>
+      <c r="C14" s="15">
+        <f t="shared" si="1"/>
+        <v>0.46666666666666662</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>2035: 0.47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>2036</v>
+      </c>
+      <c r="C15" s="15">
+        <f t="shared" si="1"/>
+        <v>0.43555555555555553</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>2036: 0.44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>2037</v>
+      </c>
+      <c r="C16" s="15">
+        <f t="shared" si="1"/>
+        <v>0.40444444444444444</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>2037: 0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>2038</v>
+      </c>
+      <c r="C17" s="15">
+        <f t="shared" si="1"/>
+        <v>0.37333333333333329</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>2038: 0.37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>2039</v>
+      </c>
+      <c r="C18" s="15">
+        <f t="shared" si="1"/>
+        <v>0.34222222222222221</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>2039: 0.34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>2040</v>
+      </c>
+      <c r="C19" s="15">
+        <f t="shared" si="1"/>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>2040: 0.31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>2041</v>
+      </c>
+      <c r="C20" s="15">
+        <f t="shared" si="1"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>2041: 0.28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>2042</v>
+      </c>
+      <c r="C21" s="15">
+        <f t="shared" si="1"/>
+        <v>0.24888888888888894</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>2042: 0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>2043</v>
+      </c>
+      <c r="C22" s="15">
+        <f t="shared" si="1"/>
+        <v>0.21777777777777774</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>2043: 0.22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>2044</v>
+      </c>
+      <c r="C23" s="15">
+        <f t="shared" si="1"/>
+        <v>0.18666666666666665</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>2044: 0.19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>2045</v>
+      </c>
+      <c r="C24" s="15">
+        <f t="shared" si="1"/>
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>2045: 0.16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>2046</v>
+      </c>
+      <c r="C25" s="15">
+        <f t="shared" si="1"/>
+        <v>0.12444444444444436</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>2046: 0.12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>2047</v>
+      </c>
+      <c r="C26" s="15">
+        <f t="shared" si="1"/>
+        <v>9.3333333333333268E-2</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>2047: 0.09</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>2048</v>
+      </c>
+      <c r="C27" s="15">
+        <f t="shared" si="1"/>
+        <v>6.2222222222222179E-2</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>2048: 0.06</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>2049</v>
+      </c>
+      <c r="C28" s="15">
+        <f t="shared" si="1"/>
+        <v>3.1111111111111089E-2</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>2049: 0.03</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>2050</v>
+      </c>
+      <c r="C29" s="15">
+        <v>0</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>2050: 0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated MDG model min capacity factor and fixed planned capacity buildout
</commit_message>
<xml_diff>
--- a/data/power-plants/mdg-power-plants.xlsx
+++ b/data/power-plants/mdg-power-plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/repositories/tza-V20/data/power-plants/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FAAAB5-7637-904E-B2F8-A380F6DD05B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C06D7A0-C0EB-5444-93F3-E2181E4A9F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{9189665D-D17D-EF4D-85B0-DA83D4B48E95}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{9189665D-D17D-EF4D-85B0-DA83D4B48E95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="67">
   <si>
     <t>Country</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>Mt</t>
+  </si>
+  <si>
+    <t>Coal and oil min CF</t>
   </si>
 </sst>
 </file>
@@ -693,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D774F4-2765-A540-807C-E0B9ADB9B465}">
   <dimension ref="A1:BF60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="AA1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="AP7" sqref="AP7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7049,373 +7052,408 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9783DCC0-9729-EA44-8E9F-A8637A17B22B}">
-  <dimension ref="A2:D29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2">
         <v>2023</v>
       </c>
       <c r="C2" s="15">
-        <v>0.84</v>
+        <v>0.5</v>
       </c>
       <c r="D2" t="str">
         <f>B2&amp;": "&amp;ROUND(C2,2)</f>
-        <v>2023: 0.84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2023: 0.5</v>
+      </c>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3">
         <v>2024</v>
       </c>
       <c r="C3" s="15">
         <f>$C$2+(($C$29-$C$2)*($B3-$B$2)/($B$29-$B$2))</f>
-        <v>0.80888888888888888</v>
+        <v>0.48148148148148151</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D29" si="0">B3&amp;": "&amp;ROUND(C3,2)</f>
-        <v>2024: 0.81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2024: 0.48</v>
+      </c>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4">
         <v>2025</v>
       </c>
       <c r="C4" s="15">
         <f t="shared" ref="C4:C28" si="1">$C$2+(($C$29-$C$2)*($B4-$B$2)/($B$29-$B$2))</f>
-        <v>0.77777777777777779</v>
+        <v>0.46296296296296297</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>2025: 0.78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2025: 0.46</v>
+      </c>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5">
         <v>2026</v>
       </c>
       <c r="C5" s="15">
         <f t="shared" si="1"/>
-        <v>0.74666666666666659</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>2026: 0.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2026: 0.44</v>
+      </c>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6">
         <v>2027</v>
       </c>
       <c r="C6" s="15">
         <f t="shared" si="1"/>
-        <v>0.7155555555555555</v>
+        <v>0.42592592592592593</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>2027: 0.72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2027: 0.43</v>
+      </c>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7">
         <v>2028</v>
       </c>
       <c r="C7" s="15">
         <f t="shared" si="1"/>
-        <v>0.68444444444444441</v>
+        <v>0.40740740740740744</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>2028: 0.68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2028: 0.41</v>
+      </c>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8">
         <v>2029</v>
       </c>
       <c r="C8" s="15">
         <f t="shared" si="1"/>
-        <v>0.65333333333333332</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>2029: 0.65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2029: 0.39</v>
+      </c>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9">
         <v>2030</v>
       </c>
       <c r="C9" s="15">
         <f t="shared" si="1"/>
-        <v>0.62222222222222223</v>
+        <v>0.37037037037037035</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>2030: 0.62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2030: 0.37</v>
+      </c>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2031</v>
       </c>
       <c r="C10" s="15">
         <f t="shared" si="1"/>
-        <v>0.59111111111111114</v>
+        <v>0.35185185185185186</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>2031: 0.59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2031: 0.35</v>
+      </c>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2032</v>
       </c>
       <c r="C11" s="15">
         <f t="shared" si="1"/>
-        <v>0.56000000000000005</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>2032: 0.56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2032: 0.33</v>
+      </c>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>2033</v>
       </c>
       <c r="C12" s="15">
         <f t="shared" si="1"/>
-        <v>0.52888888888888885</v>
+        <v>0.31481481481481483</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>2033: 0.53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2033: 0.31</v>
+      </c>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>2034</v>
       </c>
       <c r="C13" s="15">
         <f t="shared" si="1"/>
-        <v>0.49777777777777776</v>
+        <v>0.29629629629629628</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>2034: 0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2034: 0.3</v>
+      </c>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>2035</v>
       </c>
       <c r="C14" s="15">
         <f t="shared" si="1"/>
-        <v>0.46666666666666662</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>2035: 0.47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2035: 0.28</v>
+      </c>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>2036</v>
       </c>
       <c r="C15" s="15">
         <f t="shared" si="1"/>
-        <v>0.43555555555555553</v>
+        <v>0.2592592592592593</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>2036: 0.44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2036: 0.26</v>
+      </c>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>2037</v>
       </c>
       <c r="C16" s="15">
         <f t="shared" si="1"/>
-        <v>0.40444444444444444</v>
+        <v>0.24074074074074076</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>2037: 0.4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2037: 0.24</v>
+      </c>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>2038</v>
       </c>
       <c r="C17" s="15">
         <f t="shared" si="1"/>
-        <v>0.37333333333333329</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>2038: 0.37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2038: 0.22</v>
+      </c>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>2039</v>
       </c>
       <c r="C18" s="15">
         <f t="shared" si="1"/>
-        <v>0.34222222222222221</v>
+        <v>0.20370370370370372</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>2039: 0.34</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2039: 0.2</v>
+      </c>
+      <c r="F18" s="15"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>2040</v>
       </c>
       <c r="C19" s="15">
         <f t="shared" si="1"/>
-        <v>0.31111111111111112</v>
+        <v>0.18518518518518517</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>2040: 0.31</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2040: 0.19</v>
+      </c>
+      <c r="F19" s="15"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>2041</v>
       </c>
       <c r="C20" s="15">
         <f t="shared" si="1"/>
-        <v>0.28000000000000003</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>2041: 0.28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2041: 0.17</v>
+      </c>
+      <c r="F20" s="15"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>2042</v>
       </c>
       <c r="C21" s="15">
         <f t="shared" si="1"/>
-        <v>0.24888888888888894</v>
+        <v>0.14814814814814814</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>2042: 0.25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2042: 0.15</v>
+      </c>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>2043</v>
       </c>
       <c r="C22" s="15">
         <f t="shared" si="1"/>
-        <v>0.21777777777777774</v>
+        <v>0.12962962962962965</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>2043: 0.22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2043: 0.13</v>
+      </c>
+      <c r="F22" s="15"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>2044</v>
       </c>
       <c r="C23" s="15">
         <f t="shared" si="1"/>
-        <v>0.18666666666666665</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>2044: 0.19</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2044: 0.11</v>
+      </c>
+      <c r="F23" s="15"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>2045</v>
       </c>
       <c r="C24" s="15">
         <f t="shared" si="1"/>
-        <v>0.15555555555555556</v>
+        <v>9.2592592592592615E-2</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>2045: 0.16</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2045: 0.09</v>
+      </c>
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>2046</v>
       </c>
       <c r="C25" s="15">
         <f t="shared" si="1"/>
-        <v>0.12444444444444436</v>
+        <v>7.407407407407407E-2</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>2046: 0.12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2046: 0.07</v>
+      </c>
+      <c r="F25" s="15"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>2047</v>
       </c>
       <c r="C26" s="15">
         <f t="shared" si="1"/>
-        <v>9.3333333333333268E-2</v>
+        <v>5.555555555555558E-2</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>2047: 0.09</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2047: 0.06</v>
+      </c>
+      <c r="F26" s="15"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>2048</v>
       </c>
       <c r="C27" s="15">
         <f t="shared" si="1"/>
-        <v>6.2222222222222179E-2</v>
+        <v>3.7037037037037035E-2</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>2048: 0.06</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2048: 0.04</v>
+      </c>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>2049</v>
       </c>
       <c r="C28" s="15">
         <f t="shared" si="1"/>
-        <v>3.1111111111111089E-2</v>
+        <v>1.8518518518518545E-2</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>2049: 0.03</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+        <v>2049: 0.02</v>
+      </c>
+      <c r="F28" s="15"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>2050</v>
       </c>
@@ -7426,6 +7464,7 @@
         <f t="shared" si="0"/>
         <v>2050: 0</v>
       </c>
+      <c r="F29" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>